<commit_message>
Update: General.xlsx File from Crowdin
</commit_message>
<xml_diff>
--- a/ja/General.xlsx
+++ b/ja/General.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t>日本語</t>
   </si>
@@ -869,9 +869,7 @@
       <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>40</v>
       </c>

</xml_diff>